<commit_message>
add third dataset customer reviews
</commit_message>
<xml_diff>
--- a/figures.xlsx
+++ b/figures.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonwei/Desktop/nlp_augmentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAF9029-A695-FC44-ADDA-E809B8E1CE22}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AAAD14-B76D-AC41-B0E4-C4473F5DA0D3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14640" windowHeight="19900" activeTab="1" xr2:uid="{3D9FA7A2-9180-3848-8033-9AE4CD33AB87}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="14640" windowHeight="19900" activeTab="2" xr2:uid="{3D9FA7A2-9180-3848-8033-9AE4CD33AB87}"/>
   </bookViews>
   <sheets>
     <sheet name="subj" sheetId="1" r:id="rId1"/>
     <sheet name="trec" sheetId="2" r:id="rId2"/>
+    <sheet name="cr" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>% dataset</t>
   </si>
@@ -1571,8 +1572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0101491-5325-1345-A9C2-BE1B982E180C}">
   <dimension ref="A2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1679,4 +1680,118 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F0A5D5-2DB8-E045-A525-87D1F13D008E}">
+  <dimension ref="A2:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1E-3</v>
+      </c>
+      <c r="B3">
+        <v>0.53</v>
+      </c>
+      <c r="C3">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="B4">
+        <v>0.41</v>
+      </c>
+      <c r="C4">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.01</v>
+      </c>
+      <c r="B5">
+        <v>0.49</v>
+      </c>
+      <c r="C5">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.05</v>
+      </c>
+      <c r="B6">
+        <v>0.59</v>
+      </c>
+      <c r="C6">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.1</v>
+      </c>
+      <c r="B7">
+        <v>0.65</v>
+      </c>
+      <c r="C7">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.25</v>
+      </c>
+      <c r="B8">
+        <v>0.69</v>
+      </c>
+      <c r="C8">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.5</v>
+      </c>
+      <c r="B9">
+        <v>0.74</v>
+      </c>
+      <c r="C9">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0.74</v>
+      </c>
+      <c r="C10">
+        <v>0.66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add sst1 and sst2
</commit_message>
<xml_diff>
--- a/figures.xlsx
+++ b/figures.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonwei/Desktop/nlp_augmentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AAAD14-B76D-AC41-B0E4-C4473F5DA0D3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DC7115-0119-4D4A-A252-9A54392099A3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="14640" windowHeight="19900" activeTab="2" xr2:uid="{3D9FA7A2-9180-3848-8033-9AE4CD33AB87}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14640" windowHeight="19900" activeTab="3" xr2:uid="{3D9FA7A2-9180-3848-8033-9AE4CD33AB87}"/>
   </bookViews>
   <sheets>
     <sheet name="subj" sheetId="1" r:id="rId1"/>
     <sheet name="trec" sheetId="2" r:id="rId2"/>
     <sheet name="cr" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
   <si>
     <t>% dataset</t>
   </si>
@@ -1686,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F0A5D5-2DB8-E045-A525-87D1F13D008E}">
   <dimension ref="A2:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1708,10 +1709,10 @@
         <v>1E-3</v>
       </c>
       <c r="B3">
-        <v>0.53</v>
+        <v>0.64</v>
       </c>
       <c r="C3">
-        <v>0.41</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1719,10 +1720,10 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="B4">
-        <v>0.41</v>
+        <v>0.64</v>
       </c>
       <c r="C4">
-        <v>0.47</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1730,10 +1731,10 @@
         <v>0.01</v>
       </c>
       <c r="B5">
-        <v>0.49</v>
+        <v>0.67</v>
       </c>
       <c r="C5">
-        <v>0.68</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1741,10 +1742,10 @@
         <v>0.05</v>
       </c>
       <c r="B6">
-        <v>0.59</v>
+        <v>0.73</v>
       </c>
       <c r="C6">
-        <v>0.71</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1752,10 +1753,10 @@
         <v>0.1</v>
       </c>
       <c r="B7">
-        <v>0.65</v>
+        <v>0.73</v>
       </c>
       <c r="C7">
-        <v>0.76</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1763,10 +1764,10 @@
         <v>0.25</v>
       </c>
       <c r="B8">
-        <v>0.69</v>
+        <v>0.79</v>
       </c>
       <c r="C8">
-        <v>0.77</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1774,10 +1775,10 @@
         <v>0.5</v>
       </c>
       <c r="B9">
-        <v>0.74</v>
+        <v>0.81</v>
       </c>
       <c r="C9">
-        <v>0.78</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1785,10 +1786,124 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>0.74</v>
+        <v>0.83599999999999997</v>
       </c>
       <c r="C10">
-        <v>0.66</v>
+        <v>0.83799999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C1F559-E691-5943-BAA8-ECC4C4E1A177}">
+  <dimension ref="A2:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1E-3</v>
+      </c>
+      <c r="B3">
+        <v>0.254</v>
+      </c>
+      <c r="C3">
+        <v>0.26600000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="B4">
+        <v>0.214</v>
+      </c>
+      <c r="C4">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.01</v>
+      </c>
+      <c r="B5">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="C5">
+        <v>0.35899999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.05</v>
+      </c>
+      <c r="B6">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="C6">
+        <v>0.378</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.1</v>
+      </c>
+      <c r="B7">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.39900000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.25</v>
+      </c>
+      <c r="B8">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.5</v>
+      </c>
+      <c r="B9">
+        <v>0.42</v>
+      </c>
+      <c r="C9">
+        <v>0.45300000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="C10">
+        <v>0.434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>